<commit_message>
Frontend works with backend
</commit_message>
<xml_diff>
--- a/server/emails.xlsx
+++ b/server/emails.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -44,12 +44,6 @@
       <family val="1"/>
       <color theme="1"/>
       <sz val="12"/>
-    </font>
-    <font>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -88,7 +82,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -99,16 +93,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,14 +479,15 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15.6"/>
   <cols>
-    <col width="39.109375" customWidth="1" style="7" min="1" max="1"/>
-    <col width="18" customWidth="1" style="7" min="2" max="2"/>
-    <col width="8.88671875" customWidth="1" style="1" min="3" max="16384"/>
+    <col width="39.109375" customWidth="1" style="5" min="1" max="1"/>
+    <col width="18" customWidth="1" style="5" min="2" max="2"/>
+    <col width="8.88671875" customWidth="1" style="1" min="3" max="3"/>
+    <col width="8.88671875" customWidth="1" style="1" min="4" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -513,30 +503,34 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
-          <t>pratham.13jaiswal@gmail.com"</t>
+          <t>shreyaslegend364@gmail.com</t>
         </is>
       </c>
-      <c r="B2" s="5" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
-          <t>Sent Template_1</t>
+          <t>Sent</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
-          <t>instalink779@gmail.com</t>
+          <t>gowdashreyas364@gmail.com</t>
         </is>
       </c>
-      <c r="B3" s="5" t="inlineStr">
+      <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>Sent Template_1</t>
+          <t>Sent</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A3" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>